<commit_message>
Corrected Lat Lon format or changed spreadsheet tab name from Gliders to Moorings
</commit_message>
<xml_diff>
--- a/CP05MOAS-GL336/Omaha_Cal_Info_CP05MOAS-GL336_00001.xlsx
+++ b/CP05MOAS-GL336/Omaha_Cal_Info_CP05MOAS-GL336_00001.xlsx
@@ -4,38 +4,38 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19830" windowHeight="8055" tabRatio="377"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19830" windowHeight="8055" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
     <sheet name="Asset_Cal_Info" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">Asset_Cal_Info!$A$1:$F$19</definedName>
-    <definedName name="_xlnm._FilterDatabase">Asset_Cal_Info!$A$1:$F$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">Asset_Cal_Info!$A$1:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase">Asset_Cal_Info!$A$1:$F$14</definedName>
     <definedName name="_FilterDatabase_0">Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0">Moorings!$A$1:$J$97</definedName>
     <definedName name="_FilterDatabase_0_0_0">Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0_0">Moorings!$A$1:$J$97</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$413</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$408</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$413</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_1">Asset_Cal_Info!$A$1:$F$413</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$408</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_1">Asset_Cal_Info!$A$1:$F$408</definedName>
     <definedName name="_FilterDatabase_0_0_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$F$413</definedName>
+    <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$F$408</definedName>
     <definedName name="_FilterDatabase_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$F$19</definedName>
+    <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$F$14</definedName>
     <definedName name="_FilterDatabase_1_1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$97</definedName>
-    <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$413</definedName>
+    <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$408</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Ref Des</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>CP05MOAS-GL336</t>
+  </si>
+  <si>
+    <t>40°02.0500'N</t>
+  </si>
+  <si>
+    <t>70°19.7500'W</t>
   </si>
 </sst>
 </file>
@@ -344,13 +350,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -693,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -701,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,11 +783,11 @@
       <c r="F2" s="7">
         <v>42131</v>
       </c>
-      <c r="G2" s="8">
-        <v>40.034199999999998</v>
-      </c>
-      <c r="H2" s="8">
-        <v>-70.329099999999997</v>
+      <c r="G2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I2" s="4">
         <v>0</v>
@@ -790,6 +798,24 @@
       <c r="K2" s="5"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="26"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -799,10 +825,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,26 +985,33 @@
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
+    <row r="6" spans="1:16" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="14">
+        <v>336</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="15">
+        <v>2858</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="25">
+        <v>124</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:16" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="14">
@@ -991,10 +1024,10 @@
         <v>2858</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="27">
-        <v>124</v>
+        <v>21</v>
+      </c>
+      <c r="F7" s="24">
+        <v>700</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -1016,10 +1049,10 @@
         <v>2858</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" s="25">
-        <v>700</v>
+        <v>1.0760000000000001</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -1041,10 +1074,10 @@
         <v>2858</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="27">
-        <v>1.0760000000000001</v>
+        <v>23</v>
+      </c>
+      <c r="F9" s="24">
+        <v>3.9E-2</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -1052,9 +1085,9 @@
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:16" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>25</v>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="B10" s="14">
         <v>336</v>
@@ -1063,14 +1096,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="15">
-        <v>2858</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="25">
-        <v>3.9E-2</v>
-      </c>
+        <v>9030</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
@@ -1078,12 +1107,20 @@
       <c r="K10" s="20"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="26"/>
+      <c r="A11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="14">
+        <v>336</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15">
+        <v>117</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
@@ -1092,7 +1129,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="14">
         <v>336</v>
@@ -1101,7 +1138,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="15">
-        <v>9030</v>
+        <v>50152</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="22"/>
@@ -1112,10 +1149,18 @@
       <c r="K12" s="20"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
+      <c r="A13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="14">
+        <v>336</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="15">
+        <v>336</v>
+      </c>
       <c r="E13" s="20"/>
       <c r="F13" s="22"/>
       <c r="G13" s="20"/>
@@ -1124,95 +1169,6 @@
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="14">
-        <v>336</v>
-      </c>
-      <c r="C14" s="14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="15">
-        <v>117</v>
-      </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="14">
-        <v>336</v>
-      </c>
-      <c r="C16" s="14">
-        <v>1</v>
-      </c>
-      <c r="D16" s="15">
-        <v>50152</v>
-      </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="14">
-        <v>336</v>
-      </c>
-      <c r="C18" s="14">
-        <v>1</v>
-      </c>
-      <c r="D18" s="15">
-        <v>336</v>
-      </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>